<commit_message>
more inductor testing incl function generator testing
</commit_message>
<xml_diff>
--- a/eagle/inductor_test/assembly/InductorTesting.xlsx
+++ b/eagle/inductor_test/assembly/InductorTesting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24:Y24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,7 +2084,7 @@
         <v>82</v>
       </c>
       <c r="B3" t="str">
-        <f>LEFT(A3,1)</f>
+        <f t="shared" ref="B3:B40" si="0">LEFT(A3,1)</f>
         <v>C</v>
       </c>
       <c r="C3" t="s">
@@ -2096,7 +2096,7 @@
         <v>61</v>
       </c>
       <c r="B4" t="str">
-        <f>LEFT(A4,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C4" t="s">
@@ -2108,7 +2108,7 @@
         <v>67</v>
       </c>
       <c r="B5" t="str">
-        <f>LEFT(A5,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C5" t="s">
@@ -2120,7 +2120,7 @@
         <v>68</v>
       </c>
       <c r="B6" t="str">
-        <f>LEFT(A6,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C6" t="s">
@@ -2132,7 +2132,7 @@
         <v>70</v>
       </c>
       <c r="B7" t="str">
-        <f>LEFT(A7,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C7" t="s">
@@ -2144,7 +2144,7 @@
         <v>76</v>
       </c>
       <c r="B8" t="str">
-        <f>LEFT(A8,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C8" t="s">
@@ -2156,7 +2156,7 @@
         <v>83</v>
       </c>
       <c r="B9" t="str">
-        <f>LEFT(A9,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C9" t="s">
@@ -2168,7 +2168,7 @@
         <v>91</v>
       </c>
       <c r="B10" t="str">
-        <f>LEFT(A10,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C10" t="s">
@@ -2180,7 +2180,7 @@
         <v>77</v>
       </c>
       <c r="B11" t="str">
-        <f>LEFT(A11,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C11" t="s">
@@ -2192,7 +2192,7 @@
         <v>84</v>
       </c>
       <c r="B12" t="str">
-        <f>LEFT(A12,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C12" t="s">
@@ -2204,7 +2204,7 @@
         <v>60</v>
       </c>
       <c r="B13" t="str">
-        <f>LEFT(A13,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C13" t="s">
@@ -2216,7 +2216,7 @@
         <v>65</v>
       </c>
       <c r="B14" t="str">
-        <f>LEFT(A14,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C14" t="s">
@@ -2228,7 +2228,7 @@
         <v>75</v>
       </c>
       <c r="B15" t="str">
-        <f>LEFT(A15,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="C15" t="s">
@@ -2240,7 +2240,7 @@
         <v>79</v>
       </c>
       <c r="B16" t="str">
-        <f>LEFT(A16,1)</f>
+        <f t="shared" si="0"/>
         <v>L</v>
       </c>
       <c r="C16" t="s">
@@ -2252,7 +2252,7 @@
         <v>93</v>
       </c>
       <c r="B17" t="str">
-        <f>LEFT(A17,1)</f>
+        <f t="shared" si="0"/>
         <v>L</v>
       </c>
       <c r="C17" t="s">
@@ -2264,7 +2264,7 @@
         <v>71</v>
       </c>
       <c r="B18" t="str">
-        <f>LEFT(A18,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C18" t="s">
@@ -2276,7 +2276,7 @@
         <v>73</v>
       </c>
       <c r="B19" t="str">
-        <f>LEFT(A19,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C19" t="s">
@@ -2288,7 +2288,7 @@
         <v>85</v>
       </c>
       <c r="B20" t="str">
-        <f>LEFT(A20,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C20" t="s">
@@ -2300,7 +2300,7 @@
         <v>89</v>
       </c>
       <c r="B21" t="str">
-        <f>LEFT(A21,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C21" t="s">
@@ -2312,7 +2312,7 @@
         <v>90</v>
       </c>
       <c r="B22" t="str">
-        <f>LEFT(A22,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C22" t="s">
@@ -2324,7 +2324,7 @@
         <v>87</v>
       </c>
       <c r="B23" t="str">
-        <f>LEFT(A23,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C23" t="s">
@@ -2336,7 +2336,7 @@
         <v>88</v>
       </c>
       <c r="B24" t="str">
-        <f>LEFT(A24,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C24" t="s">
@@ -2348,7 +2348,7 @@
         <v>72</v>
       </c>
       <c r="B25" t="str">
-        <f>LEFT(A25,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C25" t="s">
@@ -2360,7 +2360,7 @@
         <v>81</v>
       </c>
       <c r="B26" t="str">
-        <f>LEFT(A26,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C26" t="s">
@@ -2372,7 +2372,7 @@
         <v>62</v>
       </c>
       <c r="B27" t="str">
-        <f>LEFT(A27,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C27" t="s">
@@ -2384,7 +2384,7 @@
         <v>94</v>
       </c>
       <c r="B28" t="str">
-        <f>LEFT(A28,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C28" t="s">
@@ -2396,7 +2396,7 @@
         <v>86</v>
       </c>
       <c r="B29" t="str">
-        <f>LEFT(A29,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C29" t="s">
@@ -2408,7 +2408,7 @@
         <v>64</v>
       </c>
       <c r="B30" t="str">
-        <f>LEFT(A30,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C30" t="s">
@@ -2420,7 +2420,7 @@
         <v>58</v>
       </c>
       <c r="B31" t="str">
-        <f>LEFT(A31,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C31" t="s">
@@ -2432,7 +2432,7 @@
         <v>80</v>
       </c>
       <c r="B32" t="str">
-        <f>LEFT(A32,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C32" t="s">
@@ -2444,7 +2444,7 @@
         <v>74</v>
       </c>
       <c r="B33" t="str">
-        <f>LEFT(A33,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C33" t="s">
@@ -2456,7 +2456,7 @@
         <v>63</v>
       </c>
       <c r="B34" t="str">
-        <f>LEFT(A34,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C34" t="s">
@@ -2468,7 +2468,7 @@
         <v>59</v>
       </c>
       <c r="B35" t="str">
-        <f>LEFT(A35,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="C35" t="s">
@@ -2480,7 +2480,7 @@
         <v>48</v>
       </c>
       <c r="B36" t="str">
-        <f>LEFT(A36,1)</f>
+        <f t="shared" si="0"/>
         <v>U</v>
       </c>
       <c r="C36" t="s">
@@ -2492,7 +2492,7 @@
         <v>66</v>
       </c>
       <c r="B37" t="str">
-        <f>LEFT(A37,1)</f>
+        <f t="shared" si="0"/>
         <v>U</v>
       </c>
       <c r="C37" t="s">
@@ -2504,7 +2504,7 @@
         <v>69</v>
       </c>
       <c r="B38" t="str">
-        <f>LEFT(A38,1)</f>
+        <f t="shared" si="0"/>
         <v>U</v>
       </c>
       <c r="C38" t="s">
@@ -2516,7 +2516,7 @@
         <v>78</v>
       </c>
       <c r="B39" t="str">
-        <f>LEFT(A39,1)</f>
+        <f t="shared" si="0"/>
         <v>U</v>
       </c>
       <c r="C39" t="s">
@@ -2528,7 +2528,7 @@
         <v>92</v>
       </c>
       <c r="B40" t="str">
-        <f>LEFT(A40,1)</f>
+        <f t="shared" si="0"/>
         <v>U</v>
       </c>
       <c r="C40" t="s">

</xml_diff>